<commit_message>
edit data files for test
</commit_message>
<xml_diff>
--- a/excel/EnumData.xlsx
+++ b/excel/EnumData.xlsx
@@ -8,23 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geukg\OneDrive\문서\TSomSomm\lunaria-project\lunaria-data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D03751F-FFAA-40F4-AF43-659C32F1DCC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279A8BE8-114B-4417-998B-BB4E993F4C20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3165" yWindow="3075" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="TestData" sheetId="1" r:id="rId1"/>
-    <sheet name="MapData" sheetId="2" r:id="rId2"/>
+    <sheet name="EnumData" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
-  <si>
-    <t>string</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>ColorType</t>
   </si>
@@ -36,12 +32,6 @@
   </si>
   <si>
     <t>Green</t>
-  </si>
-  <si>
-    <t>MapResourceKey</t>
-  </si>
-  <si>
-    <t>map1</t>
   </si>
   <si>
     <t>EnumName</t>
@@ -61,6 +51,10 @@
   </si>
   <si>
     <t>ResourceKey</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yellow</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -109,18 +103,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFEFEFEF"/>
-        <bgColor rgb="FFEFEFEF"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -138,12 +126,6 @@
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor rgb="FFEFEFEF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -199,25 +181,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -439,114 +419,83 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" style="14"/>
+    <col min="1" max="1" width="12.5703125" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="15"/>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15" t="s">
+      <c r="A1" s="13"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="15" t="s">
+    </row>
+    <row r="3" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="9"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="9"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="12"/>
-      <c r="B6" s="3"/>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="13"/>
+    <row r="7" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="11"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F12" s="6"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>6</v>
-      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
[Npc] CompassUI를 위한 데이터 추가3
</commit_message>
<xml_diff>
--- a/excel/EnumData.xlsx
+++ b/excel/EnumData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/geugkkom/Documents/Tsomsomm/lunaria-data/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A82A120A-5CCE-954F-B1AA-81364B6E708D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE86517-4C66-EC4C-81A1-C2B872592D97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5260" yWindow="2660" windowWidth="21600" windowHeight="11300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
   <si>
     <t>EnumName</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -129,6 +129,10 @@
   </si>
   <si>
     <t>ActivateDuration</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>PlayFixedCutscene</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -443,10 +447,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -536,18 +540,18 @@
         <v>2</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B8" s="4">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
+        <v>3</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -555,10 +559,10 @@
         <v>10</v>
       </c>
       <c r="B9" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -566,10 +570,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -577,10 +581,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="4">
-        <v>4</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>16</v>
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -588,10 +592,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="4">
-        <v>5</v>
-      </c>
-      <c r="C12" t="s">
-        <v>15</v>
+        <v>4</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -599,21 +603,21 @@
         <v>10</v>
       </c>
       <c r="B13" s="4">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="4">
         <v>6</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C14" s="7" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="4">
-        <v>1</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -621,21 +625,21 @@
         <v>17</v>
       </c>
       <c r="B15" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="8" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B16" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -643,10 +647,10 @@
         <v>22</v>
       </c>
       <c r="B17" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -654,10 +658,10 @@
         <v>22</v>
       </c>
       <c r="B18" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -665,10 +669,10 @@
         <v>22</v>
       </c>
       <c r="B19" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -676,11 +680,25 @@
         <v>22</v>
       </c>
       <c r="B20" s="4">
+        <v>4</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="4">
         <v>5</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C21" s="7" t="s">
         <v>27</v>
       </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
Revert "[Npc] 마이홈 npc"
This reverts commit 9bd4b7a9fd9c5fe19287f6d0ded74659314d046b.
</commit_message>
<xml_diff>
--- a/excel/EnumData.xlsx
+++ b/excel/EnumData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/geugkkom/Documents/Tsomsomm/lunaria-data/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D8B15A-1DA7-E94D-906F-86903107A9D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE86517-4C66-EC4C-81A1-C2B872592D97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5260" yWindow="2660" windowWidth="21600" windowHeight="11300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
   <si>
     <t>EnumName</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -133,10 +133,6 @@
   </si>
   <si>
     <t>PlayFixedCutscene</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>GoToMyhome</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -451,10 +447,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -560,13 +556,13 @@
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B9" s="4">
-        <v>4</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>30</v>
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -574,10 +570,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -585,10 +581,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -596,10 +592,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="4">
-        <v>3</v>
-      </c>
-      <c r="C12" t="s">
-        <v>14</v>
+        <v>4</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -607,10 +603,10 @@
         <v>10</v>
       </c>
       <c r="B13" s="4">
-        <v>4</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>16</v>
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -618,21 +614,21 @@
         <v>10</v>
       </c>
       <c r="B14" s="4">
-        <v>5</v>
-      </c>
-      <c r="C14" t="s">
-        <v>15</v>
+        <v>6</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="4" t="s">
-        <v>10</v>
+      <c r="A15" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="B15" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -640,21 +636,21 @@
         <v>17</v>
       </c>
       <c r="B16" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="8" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B17" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -662,10 +658,10 @@
         <v>22</v>
       </c>
       <c r="B18" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -673,10 +669,10 @@
         <v>22</v>
       </c>
       <c r="B19" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -684,10 +680,10 @@
         <v>22</v>
       </c>
       <c r="B20" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -695,25 +691,14 @@
         <v>22</v>
       </c>
       <c r="B21" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="4">
-        <v>5</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="8"/>
+      <c r="A22" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>